<commit_message>
Set up Web-App minus hosting
</commit_message>
<xml_diff>
--- a/data_pipelining/output/validated_test_leads.xlsx
+++ b/data_pipelining/output/validated_test_leads.xlsx
@@ -909,7 +909,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>anthony@fox.com</t>
+          <t>anthony.volpe@fox.com</t>
         </is>
       </c>
     </row>
@@ -1165,7 +1165,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>max@netflix.com</t>
+          <t>max.mills@netflix.com</t>
         </is>
       </c>
     </row>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>christopher@spotify.com</t>
+          <t>christopher.hill@spotify.com</t>
         </is>
       </c>
     </row>

</xml_diff>